<commit_message>
pdfs of assigm=nment 1 unit 2 lecture 3 and summary of section 3 quiz solution
</commit_message>
<xml_diff>
--- a/Quizzes and Exams (Excel Sheets)/Quizzes.xlsx
+++ b/Quizzes and Exams (Excel Sheets)/Quizzes.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Mastering-Embedded-System-Online-Diploma\Quizzes and Exams (Excel Sheets)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5F3AC6-EC03-497A-A1B0-7BC07C4E93D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="C_Basic">ورقة1!#REF!,ورقة1!$D$3</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,26 +27,205 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>C Basics</t>
+  </si>
+  <si>
+    <t>C Loops &amp; Condition</t>
+  </si>
+  <si>
+    <t>C Array &amp; String</t>
+  </si>
+  <si>
+    <t>C Functions</t>
+  </si>
+  <si>
+    <t>Mid Term 1 Exam</t>
+  </si>
+  <si>
+    <t>Structure &amp; Union &amp; Enum</t>
+  </si>
+  <si>
+    <t>Macros</t>
+  </si>
+  <si>
+    <t>C Pointers</t>
+  </si>
+  <si>
+    <t>Embedded C</t>
+  </si>
+  <si>
+    <t>Embedded C Exam</t>
+  </si>
+  <si>
+    <t>First Term Exam</t>
+  </si>
+  <si>
+    <t>Unit 5</t>
+  </si>
+  <si>
+    <t>Unit 3</t>
+  </si>
+  <si>
+    <t>Unit 2</t>
+  </si>
+  <si>
+    <t>C Array &amp; String (Quiz)</t>
+  </si>
+  <si>
+    <t>C Functions (Quiz)</t>
+  </si>
+  <si>
+    <t>Mid Term 1 Exam (Exam)</t>
+  </si>
+  <si>
+    <t>C Loops &amp; Condition (Quiz)</t>
+  </si>
+  <si>
+    <t>C Basic (Quiz)</t>
+  </si>
+  <si>
+    <t>Structure &amp; Union &amp; Enum (Quiz)</t>
+  </si>
+  <si>
+    <t>Macros (Quiz)</t>
+  </si>
+  <si>
+    <t>C Pointers (Quiz)</t>
+  </si>
+  <si>
+    <t>Embedded C (Quiz)</t>
+  </si>
+  <si>
+    <t>Embedded C Exam (Exam)</t>
+  </si>
+  <si>
+    <t>First Term Exam (Exam No.1)</t>
+  </si>
+  <si>
+    <t>First Term Exam (Exam No.2)</t>
+  </si>
+  <si>
+    <t>First Term Exam (Exam No.3)</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>(Quizzes Or Exams) HyperLniks</t>
+  </si>
+  <si>
+    <t>My Degree</t>
+  </si>
+  <si>
+    <t>Tota Degree</t>
+  </si>
+  <si>
+    <t>Date of Quiz</t>
+  </si>
+  <si>
+    <t>C Basic (Quiz) Sol</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -45,14 +233,564 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +1068,480 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="43">
+        <v>44770</v>
+      </c>
+      <c r="G1" s="44"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="13"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="31"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="26">
+        <v>60</v>
+      </c>
+      <c r="F3" s="4">
+        <v>27</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="6"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="8"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>5</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="8"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>6</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>7</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="8"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>8</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="8"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>9</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="8"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>10</v>
+      </c>
+      <c r="B12" s="34"/>
+      <c r="C12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="36">
+        <v>11</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="8"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="37"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:T2"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B3:B10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{5E4C3859-8C03-4FD2-BA1F-817143E35382}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{DE6F202B-6665-49E8-83CF-20E335AB4E9E}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{81D103DE-448D-479D-A28B-685DA10B72D7}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{1ACD564A-1440-4937-B10E-891B0FF2C0D3}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{724AA7A1-35F9-43E8-BA1E-323026B1A996}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{C078EC61-FB4A-4E56-B391-AA5EBBA68D96}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{C3989B47-8072-4050-BD83-AB3419423974}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{DA81C3C6-FCB1-4E81-8B4D-C81386571083}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{43488E0E-7B4F-41C6-B585-2831267E6CAA}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{CEE03E5C-7214-42E3-AFE5-67313C07EF85}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{01F2232B-29A7-424F-8696-4FCC13B6A426}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{D80F3C2D-0AAE-46E3-B30F-B9EC854E9005}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{75090A78-A3E1-43E3-AA4C-D7C92D2AF679}"/>
+    <hyperlink ref="G3" r:id="rId14" xr:uid="{9309498E-CD4E-4E54-8CD9-474A7DBD471A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>